<commit_message>
Updated GUI and dokumentation, listview is becoming implemented
</commit_message>
<xml_diff>
--- a/doc/10. Project Execution/Databases/SQL queries.xlsx
+++ b/doc/10. Project Execution/Databases/SQL queries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="8505"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19350" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="SQL Queries" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SQL Queries'!$A$3:$E$32</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
   <si>
     <t>Request</t>
   </si>
@@ -171,13 +171,7 @@
     <t>Titel</t>
   </si>
   <si>
-    <t>User Logout</t>
-  </si>
-  <si>
     <t xml:space="preserve">--&gt; Logout from server </t>
-  </si>
-  <si>
-    <t>Server store logout (boolean false)</t>
   </si>
   <si>
     <t>- Receive User
@@ -240,6 +234,21 @@
     <t>User Login
 Activate service go to online menu.
 User have try again.</t>
+  </si>
+  <si>
+    <t>Server store logout (boolean false)
+- Close connection/Socket</t>
+  </si>
+  <si>
+    <t>User Logout
+- Service "Log Out"
+- Close connection</t>
+  </si>
+  <si>
+    <t>SELECT ONE USER from UserID/UserName/Email - ALL DATA</t>
+  </si>
+  <si>
+    <t>UserName/Email not used earlier</t>
   </si>
 </sst>
 </file>
@@ -358,8 +367,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,7 +668,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -844,15 +853,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" ht="30">
       <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4">
@@ -1086,7 +1103,7 @@
     <sheetView showGridLines="0" topLeftCell="B4" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1124,19 +1141,19 @@
         <v>35</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -1145,37 +1162,37 @@
     <row r="6" spans="1:9" ht="105">
       <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="45">
       <c r="A7" s="8"/>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="D7" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>

</xml_diff>